<commit_message>
enhance performance of merge operations
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21210" windowHeight="10335"/>
+    <workbookView windowHeight="10335" windowWidth="21210" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="data" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>胡萝卜</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,11 +68,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>month</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#LoopFlag#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>导出时间：</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2020-12-22</t>
+    <t>operator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021-01-11</t>
   </si>
   <si>
     <t>萝卜很大</t>
@@ -253,76 +293,76 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="3" numFmtId="176" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="176" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="176" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="3" numFmtId="177" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="177" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="4" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="5" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -335,7 +375,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -351,18 +391,18 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr b="1" baseline="0" i="0" kern="1200" spc="100" strike="noStrike" sz="1600" u="none">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:outerShdw algn="t" blurRad="50800" dir="5400000" dist="38100" rotWithShape="0">
                     <a:prstClr val="black">
                       <a:alpha val="40000"/>
                     </a:prstClr>
@@ -374,10 +414,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:rPr altLang="en-US" lang="zh-CN"/>
               <a:t>全年销售额占比</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
+            <a:endParaRPr altLang="zh-CN" lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -391,18 +431,18 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr b="1" baseline="0" i="0" kern="1200" spc="100" strike="noStrike" sz="1600" u="none">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                <a:outerShdw algn="t" blurRad="50800" dir="5400000" dist="38100" rotWithShape="0">
                   <a:prstClr val="black">
                     <a:alpha val="40000"/>
                   </a:prstClr>
@@ -495,7 +535,7 @@
                 <a:noFill/>
               </a:ln>
               <a:effectLst>
-                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
                   <a:srgbClr val="000000">
                     <a:alpha val="35000"/>
                   </a:srgbClr>
@@ -505,12 +545,12 @@
                 <a:camera prst="orthographicFront">
                   <a:rot lat="0" lon="0" rev="0"/>
                 </a:camera>
-                <a:lightRig rig="threePt" dir="t">
+                <a:lightRig dir="t" rig="threePt">
                   <a:rot lat="0" lon="0" rev="1200000"/>
                 </a:lightRig>
               </a:scene3d>
               <a:sp3d>
-                <a:bevelT w="63500" h="25400"/>
+                <a:bevelT h="25400" w="63500"/>
               </a:sp3d>
             </c:spPr>
           </c:dPt>
@@ -545,7 +585,7 @@
                 <a:noFill/>
               </a:ln>
               <a:effectLst>
-                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
                   <a:srgbClr val="000000">
                     <a:alpha val="35000"/>
                   </a:srgbClr>
@@ -555,12 +595,12 @@
                 <a:camera prst="orthographicFront">
                   <a:rot lat="0" lon="0" rev="0"/>
                 </a:camera>
-                <a:lightRig rig="threePt" dir="t">
+                <a:lightRig dir="t" rig="threePt">
                   <a:rot lat="0" lon="0" rev="1200000"/>
                 </a:lightRig>
               </a:scene3d>
               <a:sp3d>
-                <a:bevelT w="63500" h="25400"/>
+                <a:bevelT h="25400" w="63500"/>
               </a:sp3d>
             </c:spPr>
           </c:dPt>
@@ -595,7 +635,7 @@
                 <a:noFill/>
               </a:ln>
               <a:effectLst>
-                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
                   <a:srgbClr val="000000">
                     <a:alpha val="35000"/>
                   </a:srgbClr>
@@ -605,12 +645,12 @@
                 <a:camera prst="orthographicFront">
                   <a:rot lat="0" lon="0" rev="0"/>
                 </a:camera>
-                <a:lightRig rig="threePt" dir="t">
+                <a:lightRig dir="t" rig="threePt">
                   <a:rot lat="0" lon="0" rev="1200000"/>
                 </a:lightRig>
               </a:scene3d>
               <a:sp3d>
-                <a:bevelT w="63500" h="25400"/>
+                <a:bevelT h="25400" w="63500"/>
               </a:sp3d>
             </c:spPr>
           </c:dPt>
@@ -623,13 +663,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr anchor="ctr" anchorCtr="1" bIns="19050" lIns="38100" rIns="38100" rot="0" spcFirstLastPara="1" tIns="19050" vert="horz" vertOverflow="ellipsis" wrap="square">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="85000"/>
@@ -694,13 +734,13 @@
                 <c:formatCode>0_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>322</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4469</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1862</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -737,11 +777,11 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="85000"/>
@@ -777,7 +817,7 @@
         </a:gs>
       </a:gsLst>
       <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
       </a:path>
       <a:tileRect/>
     </a:gradFill>
@@ -798,14 +838,14 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75" footer="0.3" header="0.3" l="0.7" r="0.7" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -821,11 +861,11 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:defRPr b="1" baseline="0" cap="none" i="0" kern="1200" strike="noStrike" sz="1400" u="none">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="85000"/>
@@ -853,11 +893,11 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+            <a:defRPr b="1" baseline="0" cap="none" i="0" kern="1200" strike="noStrike" sz="1400" u="none">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="85000"/>
@@ -893,7 +933,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln cap="rnd" w="22225">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -919,13 +959,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr anchor="ctr" anchorCtr="1" bIns="19050" lIns="38100" rIns="38100" rot="0" spcFirstLastPara="1" tIns="19050" vert="horz" vertOverflow="ellipsis" wrap="square">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
@@ -971,42 +1011,9 @@
             <c:strRef>
               <c:f>data!$C$4:$C$15</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1月</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2月</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3月</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4月</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5月</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6月</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7月</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8月</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9月</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10月</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11月</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12月</c:v>
+                  <c:v>month</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1018,40 +1025,7 @@
                 <c:formatCode>@</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1073,7 +1047,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln cap="rnd" w="22225">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -1099,13 +1073,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr anchor="ctr" anchorCtr="1" bIns="19050" lIns="38100" rIns="38100" rot="0" spcFirstLastPara="1" tIns="19050" vert="horz" vertOverflow="ellipsis" wrap="square">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
@@ -1151,42 +1125,9 @@
             <c:strRef>
               <c:f>data!$C$4:$C$15</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1月</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2月</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3月</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4月</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5月</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6月</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7月</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8月</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9月</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10月</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11月</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12月</c:v>
+                  <c:v>month</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1198,40 +1139,7 @@
                 <c:formatCode>@</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>543</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>596</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>426</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>364</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>445</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>441</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>547</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>411</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>101</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>296</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>298</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1253,7 +1161,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln cap="rnd" w="22225">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -1279,13 +1187,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr anchor="ctr" anchorCtr="1" bIns="19050" lIns="38100" rIns="38100" rot="0" spcFirstLastPara="1" tIns="19050" vert="horz" vertOverflow="ellipsis" wrap="square">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
@@ -1331,42 +1239,9 @@
             <c:strRef>
               <c:f>data!$C$4:$C$15</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1月</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2月</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3月</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4月</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5月</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6月</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7月</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8月</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9月</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10月</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11月</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12月</c:v>
+                  <c:v>month</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1378,40 +1253,7 @@
                 <c:formatCode>@</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>249</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>242</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>144</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>266</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>155</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1428,11 +1270,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="272927776"/>
-        <c:axId val="272931040"/>
+        <c:axId val="-1457861120"/>
+        <c:axId val="-1457840448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="272927776"/>
+        <c:axId val="-1457861120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1440,7 +1282,7 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
               <a:gradFill>
                 <a:gsLst>
                   <a:gs pos="100000">
@@ -1475,11 +1317,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
@@ -1493,7 +1335,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272931040"/>
+        <c:crossAx val="-1457840448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1501,7 +1343,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="272931040"/>
+        <c:axId val="-1457840448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1509,7 +1351,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
               <a:gradFill>
                 <a:gsLst>
                   <a:gs pos="100000">
@@ -1544,11 +1386,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
@@ -1562,7 +1404,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272927776"/>
+        <c:crossAx val="-1457861120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1586,11 +1428,11 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="75000"/>
@@ -1616,7 +1458,7 @@
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
       <a:solidFill>
         <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
@@ -1639,14 +1481,14 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75" footer="0.3" header="0.3" l="0.7" r="0.7" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -1662,18 +1504,18 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr b="1" baseline="0" i="0" kern="1200" spc="100" strike="noStrike" sz="1600" u="none">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:outerShdw algn="t" blurRad="50800" dir="5400000" dist="38100" rotWithShape="0">
                     <a:prstClr val="black">
                       <a:alpha val="40000"/>
                     </a:prstClr>
@@ -1685,7 +1527,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:rPr altLang="en-US" lang="zh-CN"/>
               <a:t>每月销量</a:t>
             </a:r>
             <a:endParaRPr lang="zh-CN"/>
@@ -1702,18 +1544,18 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr b="1" baseline="0" i="0" kern="1200" spc="100" strike="noStrike" sz="1600" u="none">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                <a:outerShdw algn="t" blurRad="50800" dir="5400000" dist="38100" rotWithShape="0">
                   <a:prstClr val="black">
                     <a:alpha val="40000"/>
                   </a:prstClr>
@@ -1826,7 +1668,7 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst>
-              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="35000"/>
                 </a:srgbClr>
@@ -1836,12 +1678,12 @@
               <a:camera prst="orthographicFront">
                 <a:rot lat="0" lon="0" rev="0"/>
               </a:camera>
-              <a:lightRig rig="threePt" dir="t">
+              <a:lightRig dir="t" rig="threePt">
                 <a:rot lat="0" lon="0" rev="1200000"/>
               </a:lightRig>
             </a:scene3d>
             <a:sp3d>
-              <a:bevelT w="63500" h="25400"/>
+              <a:bevelT h="25400" w="63500"/>
             </a:sp3d>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -1854,13 +1696,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr anchor="ctr" anchorCtr="1" bIns="19050" lIns="38100" rIns="38100" rot="0" spcFirstLastPara="1" tIns="19050" vert="horz" vertOverflow="ellipsis" wrap="square">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="85000"/>
@@ -1905,42 +1747,9 @@
             <c:strRef>
               <c:f>data!$C$4:$C$15</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1月</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2月</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3月</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4月</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5月</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6月</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7月</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8月</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9月</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10月</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11月</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12月</c:v>
+                  <c:v>month</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1952,40 +1761,7 @@
                 <c:formatCode>@</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2033,7 +1809,7 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst>
-              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="35000"/>
                 </a:srgbClr>
@@ -2043,12 +1819,12 @@
               <a:camera prst="orthographicFront">
                 <a:rot lat="0" lon="0" rev="0"/>
               </a:camera>
-              <a:lightRig rig="threePt" dir="t">
+              <a:lightRig dir="t" rig="threePt">
                 <a:rot lat="0" lon="0" rev="1200000"/>
               </a:lightRig>
             </a:scene3d>
             <a:sp3d>
-              <a:bevelT w="63500" h="25400"/>
+              <a:bevelT h="25400" w="63500"/>
             </a:sp3d>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -2061,13 +1837,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr anchor="ctr" anchorCtr="1" bIns="19050" lIns="38100" rIns="38100" rot="0" spcFirstLastPara="1" tIns="19050" vert="horz" vertOverflow="ellipsis" wrap="square">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="85000"/>
@@ -2112,42 +1888,9 @@
             <c:strRef>
               <c:f>data!$C$4:$C$15</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1月</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2月</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3月</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4月</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5月</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6月</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7月</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8月</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9月</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10月</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11月</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12月</c:v>
+                  <c:v>month</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2159,40 +1902,7 @@
                 <c:formatCode>@</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>543</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>596</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>426</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>364</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>445</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>441</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>547</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>411</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>101</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>296</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>298</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2240,7 +1950,7 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst>
-              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="35000"/>
                 </a:srgbClr>
@@ -2250,12 +1960,12 @@
               <a:camera prst="orthographicFront">
                 <a:rot lat="0" lon="0" rev="0"/>
               </a:camera>
-              <a:lightRig rig="threePt" dir="t">
+              <a:lightRig dir="t" rig="threePt">
                 <a:rot lat="0" lon="0" rev="1200000"/>
               </a:lightRig>
             </a:scene3d>
             <a:sp3d>
-              <a:bevelT w="63500" h="25400"/>
+              <a:bevelT h="25400" w="63500"/>
             </a:sp3d>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -2263,42 +1973,9 @@
             <c:strRef>
               <c:f>data!$C$4:$C$15</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1月</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2月</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3月</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4月</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5月</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6月</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7月</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8月</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9月</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10月</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11月</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12月</c:v>
+                  <c:v>month</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2310,40 +1987,7 @@
                 <c:formatCode>@</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>249</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>242</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>144</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>266</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>155</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2359,12 +2003,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="272940288"/>
-        <c:axId val="272934848"/>
+        <c:axId val="-1457836640"/>
+        <c:axId val="-1457857312"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="272940288"/>
+        <c:axId val="-1457836640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2382,11 +2026,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="85000"/>
@@ -2400,7 +2044,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272934848"/>
+        <c:crossAx val="-1457857312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2408,7 +2052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="272934848"/>
+        <c:axId val="-1457857312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2416,7 +2060,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
               <a:solidFill>
                 <a:schemeClr val="dk1">
                   <a:lumMod val="50000"/>
@@ -2440,11 +2084,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="85000"/>
@@ -2458,7 +2102,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272940288"/>
+        <c:crossAx val="-1457836640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2482,11 +2126,11 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="85000"/>
@@ -2522,7 +2166,7 @@
         </a:gs>
       </a:gsLst>
       <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
       </a:path>
       <a:tileRect/>
     </a:gradFill>
@@ -2543,7 +2187,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75" footer="0.3" header="0.3" l="0.7" r="0.7" t="0.75"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4191,7 +3835,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
@@ -4296,10 +3940,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -4334,7 +3978,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4369,7 +4013,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4457,7 +4101,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -4466,13 +4110,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -4482,7 +4126,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -4491,7 +4135,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -4500,7 +4144,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -4510,12 +4154,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -4546,7 +4190,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -4565,7 +4209,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -4577,32 +4221,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="14" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="14.25" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="14" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.25" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.75" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.75" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="15.125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="18.125" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" style="1" width="14.0" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" style="1" width="14.25" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" style="1" width="14.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="13.25" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="12.75" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="13.75" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="53.25" r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
@@ -4620,12 +4262,12 @@
       </c>
       <c r="I1" s="22"/>
     </row>
-    <row r="2" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="53.25" r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="10" t="s">
@@ -4650,340 +4292,340 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="42.75" r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="11" t="e">
         <f>AVERAGE(D4:D25)</f>
-        <v>36.900199454959598</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E3" s="4">
         <f>SUM(E4:E25)</f>
-        <v>322</v>
-      </c>
-      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="e">
         <f>AVERAGE(F4:F25)</f>
-        <v>106.85859561099829</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G3" s="4">
         <f>SUM(G4:G25)</f>
-        <v>4469</v>
-      </c>
-      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4" t="e">
         <f>AVERAGE(H4:H25)</f>
-        <v>15.513300593840183</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="I3" s="4">
         <f>SUM(I4:I25)</f>
-        <v>1862</v>
-      </c>
-      <c r="J3" s="11">
+        <v>0</v>
+      </c>
+      <c r="J3" s="11" t="e">
         <f>D3*E3+F3*G3+H3*I3</f>
-        <v>518318.69371577876</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4">
       <c r="C4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="14">
-        <v>13.371581542606686</v>
-      </c>
-      <c r="E4" s="14">
-        <v>66</v>
-      </c>
-      <c r="F4" s="14">
-        <v>95.01142041394958</v>
-      </c>
-      <c r="G4" s="14">
-        <v>543</v>
-      </c>
-      <c r="H4" s="14">
-        <v>20.415817822617043</v>
-      </c>
-      <c r="I4" s="14">
-        <v>249</v>
+        <v>26</v>
+      </c>
+      <c r="D4" s="14" t="n">
+        <v>51.770907643488</v>
+      </c>
+      <c r="E4" s="14" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="F4" s="14" t="n">
+        <v>3.779187243024677</v>
+      </c>
+      <c r="G4" s="14" t="n">
+        <v>585.0</v>
+      </c>
+      <c r="H4" s="14" t="n">
+        <v>29.918763317971507</v>
+      </c>
+      <c r="I4" s="14" t="n">
+        <v>249.0</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5">
       <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="14">
-        <v>9.261564449775058</v>
-      </c>
-      <c r="E5" s="14">
-        <v>1</v>
-      </c>
-      <c r="F5" s="14">
-        <v>172.18250851425933</v>
-      </c>
-      <c r="G5" s="14">
-        <v>596</v>
-      </c>
-      <c r="H5" s="14">
-        <v>21.04870310203831</v>
-      </c>
-      <c r="I5" s="14">
         <v>27</v>
+      </c>
+      <c r="D5" s="14" t="n">
+        <v>16.1890817198666</v>
+      </c>
+      <c r="E5" s="14" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="F5" s="14" t="n">
+        <v>57.2267239689793</v>
+      </c>
+      <c r="G5" s="14" t="n">
+        <v>443.0</v>
+      </c>
+      <c r="H5" s="14" t="n">
+        <v>42.81109579543078</v>
+      </c>
+      <c r="I5" s="14" t="n">
+        <v>8.0</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6">
       <c r="C6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="14">
-        <v>52.765645366227915</v>
-      </c>
-      <c r="E6" s="14">
-        <v>24</v>
-      </c>
-      <c r="F6" s="14">
-        <v>158.41191991108118</v>
-      </c>
-      <c r="G6" s="14">
-        <v>1</v>
-      </c>
-      <c r="H6" s="14">
-        <v>23.066897127274189</v>
-      </c>
-      <c r="I6" s="14">
-        <v>242</v>
+        <v>28</v>
+      </c>
+      <c r="D6" s="14" t="n">
+        <v>34.865603386588404</v>
+      </c>
+      <c r="E6" s="14" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="F6" s="14" t="n">
+        <v>5.930332835531042</v>
+      </c>
+      <c r="G6" s="14" t="n">
+        <v>467.0</v>
+      </c>
+      <c r="H6" s="14" t="n">
+        <v>19.14982628027355</v>
+      </c>
+      <c r="I6" s="14" t="n">
+        <v>241.0</v>
       </c>
       <c r="J6" s="15"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7">
       <c r="C7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="14">
-        <v>10.456414817454196</v>
-      </c>
-      <c r="E7" s="14">
-        <v>9</v>
-      </c>
-      <c r="F7" s="14">
-        <v>1.90746384868269</v>
-      </c>
-      <c r="G7" s="14">
-        <v>426</v>
-      </c>
-      <c r="H7" s="14">
-        <v>6.7588782982059668</v>
-      </c>
-      <c r="I7" s="14">
-        <v>144</v>
+        <v>29</v>
+      </c>
+      <c r="D7" s="14" t="n">
+        <v>62.96257363175009</v>
+      </c>
+      <c r="E7" s="14" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="F7" s="14" t="n">
+        <v>143.50191413190825</v>
+      </c>
+      <c r="G7" s="14" t="n">
+        <v>475.0</v>
+      </c>
+      <c r="H7" s="14" t="n">
+        <v>42.258868348470855</v>
+      </c>
+      <c r="I7" s="14" t="n">
+        <v>95.0</v>
       </c>
       <c r="J7" s="15"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8">
       <c r="C8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="14">
-        <v>49.607151568164021</v>
-      </c>
-      <c r="E8" s="14">
-        <v>14</v>
-      </c>
-      <c r="F8" s="14">
-        <v>12.62255474779151</v>
-      </c>
-      <c r="G8" s="14">
-        <v>364</v>
-      </c>
-      <c r="H8" s="14">
-        <v>3.418178690580258</v>
-      </c>
-      <c r="I8" s="14">
-        <v>52</v>
+        <v>30</v>
+      </c>
+      <c r="D8" s="14" t="n">
+        <v>19.889574198994808</v>
+      </c>
+      <c r="E8" s="14" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="F8" s="14" t="n">
+        <v>149.75682073444975</v>
+      </c>
+      <c r="G8" s="14" t="n">
+        <v>554.0</v>
+      </c>
+      <c r="H8" s="14" t="n">
+        <v>22.46973573891287</v>
+      </c>
+      <c r="I8" s="14" t="n">
+        <v>262.0</v>
       </c>
       <c r="J8" s="15"/>
       <c r="K8" s="16"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9">
       <c r="C9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="14">
-        <v>20.656763797586294</v>
-      </c>
-      <c r="E9" s="14">
-        <v>18</v>
-      </c>
-      <c r="F9" s="14">
-        <v>33.133019683428387</v>
-      </c>
-      <c r="G9" s="14">
-        <v>445</v>
-      </c>
-      <c r="H9" s="14">
-        <v>20.180698920153905</v>
-      </c>
-      <c r="I9" s="14">
-        <v>195</v>
+        <v>31</v>
+      </c>
+      <c r="D9" s="14" t="n">
+        <v>8.652804050308568</v>
+      </c>
+      <c r="E9" s="14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F9" s="14" t="n">
+        <v>119.30554915254275</v>
+      </c>
+      <c r="G9" s="14" t="n">
+        <v>601.0</v>
+      </c>
+      <c r="H9" s="14" t="n">
+        <v>7.364525953548196</v>
+      </c>
+      <c r="I9" s="14" t="n">
+        <v>220.0</v>
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="16"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10">
       <c r="C10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="14">
-        <v>59.489852443069395</v>
-      </c>
-      <c r="E10" s="14">
-        <v>0</v>
-      </c>
-      <c r="F10" s="14">
-        <v>165.67315815335564</v>
-      </c>
-      <c r="G10" s="14">
-        <v>441</v>
-      </c>
-      <c r="H10" s="14">
-        <v>22.796120256235053</v>
-      </c>
-      <c r="I10" s="14">
-        <v>218</v>
+        <v>32</v>
+      </c>
+      <c r="D10" s="14" t="n">
+        <v>2.093522821491483</v>
+      </c>
+      <c r="E10" s="14" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="F10" s="14" t="n">
+        <v>54.29677905940273</v>
+      </c>
+      <c r="G10" s="14" t="n">
+        <v>602.0</v>
+      </c>
+      <c r="H10" s="14" t="n">
+        <v>29.657148134498776</v>
+      </c>
+      <c r="I10" s="14" t="n">
+        <v>218.0</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="16"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11">
       <c r="C11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="14">
-        <v>51.552079512773005</v>
-      </c>
-      <c r="E11" s="14">
-        <v>11</v>
-      </c>
-      <c r="F11" s="14">
-        <v>92.069095785918748</v>
-      </c>
-      <c r="G11" s="14">
-        <v>547</v>
-      </c>
-      <c r="H11" s="14">
-        <v>14.402507778432831</v>
-      </c>
-      <c r="I11" s="14">
-        <v>232</v>
+        <v>33</v>
+      </c>
+      <c r="D11" s="14" t="n">
+        <v>47.97203229235001</v>
+      </c>
+      <c r="E11" s="14" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="F11" s="14" t="n">
+        <v>94.25180927462719</v>
+      </c>
+      <c r="G11" s="14" t="n">
+        <v>326.0</v>
+      </c>
+      <c r="H11" s="14" t="n">
+        <v>17.71348947458766</v>
+      </c>
+      <c r="I11" s="14" t="n">
+        <v>113.0</v>
       </c>
       <c r="J11" s="15"/>
       <c r="K11" s="16"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12">
       <c r="C12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="14">
-        <v>11.727517357914792</v>
-      </c>
-      <c r="E12" s="14">
-        <v>28</v>
-      </c>
-      <c r="F12" s="14">
-        <v>165.30789710621758</v>
-      </c>
-      <c r="G12" s="14">
-        <v>411</v>
-      </c>
-      <c r="H12" s="14">
-        <v>13.833800778182852</v>
-      </c>
-      <c r="I12" s="14">
-        <v>266</v>
+        <v>34</v>
+      </c>
+      <c r="D12" s="14" t="n">
+        <v>7.6895749100910615</v>
+      </c>
+      <c r="E12" s="14" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="F12" s="14" t="n">
+        <v>7.368976908940475</v>
+      </c>
+      <c r="G12" s="14" t="n">
+        <v>525.0</v>
+      </c>
+      <c r="H12" s="14" t="n">
+        <v>14.264113169648962</v>
+      </c>
+      <c r="I12" s="14" t="n">
+        <v>177.0</v>
       </c>
       <c r="J12" s="15"/>
       <c r="K12" s="16"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13">
       <c r="C13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="14">
-        <v>46.322891895146839</v>
-      </c>
-      <c r="E13" s="14">
-        <v>7</v>
-      </c>
-      <c r="F13" s="14">
-        <v>108.86611131491073</v>
-      </c>
-      <c r="G13" s="14">
-        <v>101</v>
-      </c>
-      <c r="H13" s="14">
-        <v>23.497635401932122</v>
-      </c>
-      <c r="I13" s="14">
-        <v>25</v>
+        <v>35</v>
+      </c>
+      <c r="D13" s="14" t="n">
+        <v>19.413483175636713</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="F13" s="14" t="n">
+        <v>91.54756804917443</v>
+      </c>
+      <c r="G13" s="14" t="n">
+        <v>242.0</v>
+      </c>
+      <c r="H13" s="14" t="n">
+        <v>24.89281261926465</v>
+      </c>
+      <c r="I13" s="14" t="n">
+        <v>222.0</v>
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="16"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14">
       <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="14">
-        <v>56.996014477215567</v>
-      </c>
-      <c r="E14" s="14">
-        <v>76</v>
-      </c>
-      <c r="F14" s="14">
-        <v>145.18453665114941</v>
-      </c>
-      <c r="G14" s="14">
-        <v>296</v>
-      </c>
-      <c r="H14" s="14">
-        <v>11.677497155325112</v>
-      </c>
-      <c r="I14" s="14">
-        <v>57</v>
+        <v>36</v>
+      </c>
+      <c r="D14" s="14" t="n">
+        <v>24.04298275497596</v>
+      </c>
+      <c r="E14" s="14" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="F14" s="14" t="n">
+        <v>68.42584415275893</v>
+      </c>
+      <c r="G14" s="14" t="n">
+        <v>435.0</v>
+      </c>
+      <c r="H14" s="14" t="n">
+        <v>5.277532011778943</v>
+      </c>
+      <c r="I14" s="14" t="n">
+        <v>229.0</v>
       </c>
       <c r="J14" s="15"/>
       <c r="K14" s="16"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15">
       <c r="C15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="14">
-        <v>60.594916231581408</v>
-      </c>
-      <c r="E15" s="14">
-        <v>68</v>
-      </c>
-      <c r="F15" s="14">
-        <v>131.93346120123468</v>
-      </c>
-      <c r="G15" s="14">
-        <v>298</v>
-      </c>
-      <c r="H15" s="14">
-        <v>5.0628717951045745</v>
-      </c>
-      <c r="I15" s="14">
-        <v>155</v>
+        <v>37</v>
+      </c>
+      <c r="D15" s="14" t="n">
+        <v>45.38692115455145</v>
+      </c>
+      <c r="E15" s="14" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="F15" s="14" t="n">
+        <v>2.314368768090385</v>
+      </c>
+      <c r="G15" s="14" t="n">
+        <v>317.0</v>
+      </c>
+      <c r="H15" s="14" t="n">
+        <v>13.366202671283098</v>
+      </c>
+      <c r="I15" s="14" t="n">
+        <v>26.0</v>
       </c>
       <c r="J15" s="15"/>
       <c r="K15" s="16"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.15">
       <c r="C16" s="6"/>
       <c r="D16" s="13"/>
       <c r="E16" s="7"/>
@@ -5149,7 +4791,7 @@
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.15">
+    <row r="32" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
@@ -5195,14 +4837,15 @@
       <c r="I36" s="7"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="true"/>
   <mergeCells count="3">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>